<commit_message>
Adding hibernate employees table
</commit_message>
<xml_diff>
--- a/DataDictionaryWedding.xlsx
+++ b/DataDictionaryWedding.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Awaab\Revature\Projects\p1\AG_P1_AwaabGurman\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{14E76C6B-275B-4EA1-9D5B-448251CFEF23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{361B5F99-3A1C-4305-A62E-0214F2B26F26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23550" yWindow="1230" windowWidth="20085" windowHeight="11805" xr2:uid="{A8AB1134-95D0-4A3A-8860-45946E82E881}"/>
+    <workbookView xWindow="-38510" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{A8AB1134-95D0-4A3A-8860-45946E82E881}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1 (2)" sheetId="3" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1046" uniqueCount="156">
   <si>
     <t>display name​</t>
   </si>
@@ -488,6 +489,33 @@
   </si>
   <si>
     <t>confirmation of plus one attendee</t>
+  </si>
+  <si>
+    <t>employee_type_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fk from </t>
+  </si>
+  <si>
+    <t>employee_type.employee_type_id</t>
+  </si>
+  <si>
+    <t>employee_type</t>
+  </si>
+  <si>
+    <t>primary key of employee_type</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>description of the type (musicians,carterer,photographers,florists)</t>
+  </si>
+  <si>
+    <t>tracking bethrotheds</t>
   </si>
 </sst>
 </file>
@@ -523,7 +551,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -545,6 +573,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -613,7 +647,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -635,6 +669,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -949,11 +998,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C53AC00D-D810-40C7-9987-306738D63BFC}">
-  <dimension ref="A1:I98"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D772D798-FF15-4D71-86C4-88DA9269BE37}">
+  <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="I99" sqref="I99"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1146,6 +1195,1378 @@
         <v>23</v>
       </c>
     </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C13" s="4">
+        <v>255</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="12"/>
+    </row>
+    <row r="15" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="4">
+        <v>40</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="4">
+        <v>40</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="4">
+        <v>40</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="4">
+        <v>40</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="8"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C37" s="4">
+        <v>40</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I37" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A40" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I40" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H41" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I41" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C42" s="4">
+        <v>40</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H42" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I42" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C43" s="4">
+        <v>40</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G43" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H43" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I43" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A46" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I46" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A47" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G47" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H47" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I47" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A48" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C48" s="4">
+        <v>40</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G48" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H48" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I48" s="4"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A49" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G49" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H49" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I49" s="4"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A50" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C50" s="4">
+        <v>40</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F50" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G50" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H50" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I50" s="4"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A51" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C51" s="4">
+        <v>40</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G51" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H51" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I51" s="4"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A54" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H54" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I54" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A55" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G55" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H55" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="I55" s="5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A56" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G56" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H56" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="I56" s="6"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A57" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G57" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H57" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="I57" s="7"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A58" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F58" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G58" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H58" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I58" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A59" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F59" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G59" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H59" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I59" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A60" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="E60" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F60" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G60" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H60" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I60" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="I55:I57"/>
+    <mergeCell ref="I13:I14"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C53AC00D-D810-40C7-9987-306738D63BFC}">
+  <dimension ref="A1:I98"/>
+  <sheetViews>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="8.88671875" style="2"/>
+    <col min="8" max="8" width="28.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="4">
+        <v>40</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="4">
+        <v>40</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="4">
+        <v>40</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="4">
+        <v>40</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>31</v>
@@ -3252,7 +4673,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9DFBFBB-EDB8-453B-A551-B329BA46ACF7}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>